<commit_message>
added examples and removed unecessary files
</commit_message>
<xml_diff>
--- a/Data_inputs.xlsx
+++ b/Data_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ek2517/Documents/GitHub/ARIA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E69B793-16A5-A94E-B4AD-18F5CFE4A01B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0BFB69-5AB9-0947-B466-C0B90CEA42D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17740" xr2:uid="{3367ADF2-404E-8249-84D1-C6000992A6DA}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" xr2:uid="{3367ADF2-404E-8249-84D1-C6000992A6DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Input/output</t>
   </si>
@@ -44,37 +44,7 @@
     <t>In/out</t>
   </si>
   <si>
-    <t>Sodium hydroxide</t>
-  </si>
-  <si>
-    <t>Copper</t>
-  </si>
-  <si>
-    <t>Cobalt sulfate</t>
-  </si>
-  <si>
-    <t>Nickel sulfate</t>
-  </si>
-  <si>
-    <t>Manganese sulphate</t>
-  </si>
-  <si>
-    <t>Graphite</t>
-  </si>
-  <si>
     <t>Units</t>
-  </si>
-  <si>
-    <t>kg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kg </t>
-  </si>
-  <si>
-    <t>Electricity</t>
-  </si>
-  <si>
-    <t>kWh</t>
   </si>
 </sst>
 </file>
@@ -483,7 +453,7 @@
   <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A2" sqref="A2:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -499,244 +469,233 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
-        <v>1.7229103949362945</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.33002498263446767</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.95381130642672352</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0.92930694082929721</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0.95229034580343486</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0.90299487083526231</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
+      <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
+      <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
+      <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added ballpoint example and updaed code
</commit_message>
<xml_diff>
--- a/Data_inputs.xlsx
+++ b/Data_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ek2517/Documents/GitHub/ARIA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0BFB69-5AB9-0947-B466-C0B90CEA42D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{50F8E795-36AB-3D4B-A2A3-B6A71F6BC652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" xr2:uid="{3367ADF2-404E-8249-84D1-C6000992A6DA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Input/output</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Units</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -450,19 +453,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F7873A-0819-734F-9E17-474161EBC605}">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C8"/>
+      <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.1640625" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" customWidth="1"/>
+    <col min="1" max="1" width="40.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,260 +476,54 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" s="2"/>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" s="2"/>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" s="2"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="2"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="2"/>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="2"/>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="2"/>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="2"/>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="2"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="2"/>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="2"/>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>